<commit_message>
Added new motors and propellers
Double checked Georgia's motor data and added it to Import Data. Added Judah's and Lucy's propellers. Corrected datasheets with missing data. Created a folder to contain old DataImport.mat files so we can store old DataImport.mat files in case the new one is inaccurate
</commit_message>
<xml_diff>
--- a/Import Data/14x11.xlsx
+++ b/Import Data/14x11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe1ca5d0fde44768/Documents/UCSD/dbf-propulsions/Import Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\GitHub\dbf-propulsions\Import Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE5D89D4-B6DD-426F-B694-F7549C18A0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E9EE11-6452-4FE9-80DF-CAD45C7A1582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="2244" windowWidth="20736" windowHeight="10440" xr2:uid="{4AEDA0A7-0E86-4334-8F64-2D5D76479C10}"/>
+    <workbookView xWindow="23700" yWindow="4455" windowWidth="14130" windowHeight="14790" xr2:uid="{4AEDA0A7-0E86-4334-8F64-2D5D76479C10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,30 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="46">
   <si>
     <t>14x11</t>
   </si>
@@ -196,15 +174,6 @@
   </si>
   <si>
     <t>(Lbf)</t>
-  </si>
-  <si>
-    <t>0.87-NaN</t>
-  </si>
-  <si>
-    <t>0.90-NaN</t>
-  </si>
-  <si>
-    <t>0.94-NaN</t>
   </si>
 </sst>
 </file>
@@ -559,13 +528,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DBCF8E3-231A-4A75-9BC8-8A832EB761C1}">
   <dimension ref="A1:I565"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
+      <selection activeCell="B522" sqref="B522"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +545,7 @@
         <v>41994</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -605,12 +574,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -621,7 +590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -644,7 +613,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -667,7 +636,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -675,7 +644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -692,7 +661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -706,7 +675,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -732,7 +701,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -752,7 +721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -778,7 +747,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.5</v>
       </c>
@@ -804,7 +773,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -830,7 +799,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.4</v>
       </c>
@@ -856,7 +825,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.9</v>
       </c>
@@ -882,7 +851,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2.4</v>
       </c>
@@ -908,7 +877,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2.9</v>
       </c>
@@ -934,7 +903,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3.4</v>
       </c>
@@ -960,7 +929,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3.9</v>
       </c>
@@ -986,7 +955,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4.3</v>
       </c>
@@ -1012,7 +981,7 @@
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4.8</v>
       </c>
@@ -1038,7 +1007,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5.3</v>
       </c>
@@ -1064,7 +1033,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5.8</v>
       </c>
@@ -1090,7 +1059,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6.3</v>
       </c>
@@ -1116,7 +1085,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6.8</v>
       </c>
@@ -1142,7 +1111,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.2</v>
       </c>
@@ -1168,7 +1137,7 @@
         <v>0.114</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.7</v>
       </c>
@@ -1194,7 +1163,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8.1999999999999993</v>
       </c>
@@ -1220,7 +1189,7 @@
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8.6999999999999993</v>
       </c>
@@ -1246,7 +1215,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9.1999999999999993</v>
       </c>
@@ -1272,7 +1241,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9.6999999999999993</v>
       </c>
@@ -1298,7 +1267,7 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10.1</v>
       </c>
@@ -1324,7 +1293,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10.6</v>
       </c>
@@ -1350,7 +1319,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>11.1</v>
       </c>
@@ -1376,7 +1345,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>11.6</v>
       </c>
@@ -1402,7 +1371,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12.1</v>
       </c>
@@ -1428,7 +1397,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>12.6</v>
       </c>
@@ -1454,7 +1423,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>13</v>
       </c>
@@ -1480,7 +1449,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>13.5</v>
       </c>
@@ -1506,7 +1475,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14</v>
       </c>
@@ -1532,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -1546,7 +1515,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1572,7 +1541,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>40</v>
       </c>
@@ -1592,7 +1561,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -1618,7 +1587,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1644,7 +1613,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1.9</v>
       </c>
@@ -1670,7 +1639,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2.9</v>
       </c>
@@ -1696,7 +1665,7 @@
         <v>0.54300000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3.9</v>
       </c>
@@ -1722,7 +1691,7 @@
         <v>0.54300000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4.8</v>
       </c>
@@ -1748,7 +1717,7 @@
         <v>0.54300000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5.8</v>
       </c>
@@ -1774,7 +1743,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6.8</v>
       </c>
@@ -1800,7 +1769,7 @@
         <v>0.54100000000000004</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7.7</v>
       </c>
@@ -1826,7 +1795,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>8.6999999999999993</v>
       </c>
@@ -1852,7 +1821,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9.6999999999999993</v>
       </c>
@@ -1878,7 +1847,7 @@
         <v>0.52900000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>10.6</v>
       </c>
@@ -1904,7 +1873,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>11.6</v>
       </c>
@@ -1930,7 +1899,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>12.6</v>
       </c>
@@ -1956,7 +1925,7 @@
         <v>0.49399999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>13.5</v>
       </c>
@@ -1982,7 +1951,7 @@
         <v>0.47599999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>14.5</v>
       </c>
@@ -2008,7 +1977,7 @@
         <v>0.45500000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>15.5</v>
       </c>
@@ -2034,7 +2003,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>16.399999999999999</v>
       </c>
@@ -2060,7 +2029,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>17.399999999999999</v>
       </c>
@@ -2086,7 +2055,7 @@
         <v>0.376</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>18.3</v>
       </c>
@@ -2112,7 +2081,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>19.3</v>
       </c>
@@ -2138,7 +2107,7 @@
         <v>0.314</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>20.3</v>
       </c>
@@ -2164,7 +2133,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>21.2</v>
       </c>
@@ -2190,7 +2159,7 @@
         <v>0.249</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>22.2</v>
       </c>
@@ -2216,7 +2185,7 @@
         <v>0.215</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>23.2</v>
       </c>
@@ -2242,7 +2211,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>24.1</v>
       </c>
@@ -2268,7 +2237,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>25.1</v>
       </c>
@@ -2294,7 +2263,7 @@
         <v>0.109</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>26.1</v>
       </c>
@@ -2320,7 +2289,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>27</v>
       </c>
@@ -2346,7 +2315,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>28</v>
       </c>
@@ -2372,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>30</v>
       </c>
@@ -2386,7 +2355,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>26</v>
       </c>
@@ -2412,7 +2381,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>40</v>
       </c>
@@ -2432,7 +2401,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -2458,7 +2427,7 @@
         <v>1.216</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1.4</v>
       </c>
@@ -2484,7 +2453,7 @@
         <v>1.2170000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2.9</v>
       </c>
@@ -2510,7 +2479,7 @@
         <v>1.2170000000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4.3</v>
       </c>
@@ -2536,7 +2505,7 @@
         <v>1.218</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5.8</v>
       </c>
@@ -2562,7 +2531,7 @@
         <v>1.2190000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>7.2</v>
       </c>
@@ -2588,7 +2557,7 @@
         <v>1.2190000000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>8.6999999999999993</v>
       </c>
@@ -2614,7 +2583,7 @@
         <v>1.218</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>10.1</v>
       </c>
@@ -2640,7 +2609,7 @@
         <v>1.2150000000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>11.6</v>
       </c>
@@ -2666,7 +2635,7 @@
         <v>1.2110000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>13</v>
       </c>
@@ -2692,7 +2661,7 @@
         <v>1.202</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>14.5</v>
       </c>
@@ -2718,7 +2687,7 @@
         <v>1.1879999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>15.9</v>
       </c>
@@ -2744,7 +2713,7 @@
         <v>1.169</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>17.399999999999999</v>
       </c>
@@ -2770,7 +2739,7 @@
         <v>1.143</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>18.8</v>
       </c>
@@ -2796,7 +2765,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>20.3</v>
       </c>
@@ -2822,7 +2791,7 @@
         <v>1.071</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>21.7</v>
       </c>
@@ -2848,7 +2817,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>23.2</v>
       </c>
@@ -2874,7 +2843,7 @@
         <v>0.97299999999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>24.6</v>
       </c>
@@ -2900,7 +2869,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>26.1</v>
       </c>
@@ -2926,7 +2895,7 @@
         <v>0.84899999999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>27.5</v>
       </c>
@@ -2952,7 +2921,7 @@
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>29</v>
       </c>
@@ -2978,7 +2947,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>30.4</v>
       </c>
@@ -3004,7 +2973,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>31.9</v>
       </c>
@@ -3030,7 +2999,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>33.299999999999997</v>
       </c>
@@ -3056,7 +3025,7 @@
         <v>0.48399999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>34.700000000000003</v>
       </c>
@@ -3082,7 +3051,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>36.200000000000003</v>
       </c>
@@ -3108,7 +3077,7 @@
         <v>0.32700000000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>37.6</v>
       </c>
@@ -3134,7 +3103,7 @@
         <v>0.246</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>39.1</v>
       </c>
@@ -3160,7 +3129,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>40.5</v>
       </c>
@@ -3186,7 +3155,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>42</v>
       </c>
@@ -3212,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>30</v>
       </c>
@@ -3226,7 +3195,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -3252,7 +3221,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>40</v>
       </c>
@@ -3272,7 +3241,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0</v>
       </c>
@@ -3298,7 +3267,7 @@
         <v>2.1520000000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1.9</v>
       </c>
@@ -3324,7 +3293,7 @@
         <v>2.1539999999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>3.9</v>
       </c>
@@ -3350,7 +3319,7 @@
         <v>2.1560000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>5.8</v>
       </c>
@@ -3376,7 +3345,7 @@
         <v>2.157</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>7.7</v>
       </c>
@@ -3402,7 +3371,7 @@
         <v>2.1579999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>9.6999999999999993</v>
       </c>
@@ -3428,7 +3397,7 @@
         <v>2.1579999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>11.6</v>
       </c>
@@ -3454,7 +3423,7 @@
         <v>2.157</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>13.5</v>
       </c>
@@ -3480,7 +3449,7 @@
         <v>2.1539999999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>15.4</v>
       </c>
@@ -3506,7 +3475,7 @@
         <v>2.1469999999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>17.399999999999999</v>
       </c>
@@ -3532,7 +3501,7 @@
         <v>2.1339999999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>19.3</v>
       </c>
@@ -3558,7 +3527,7 @@
         <v>2.1110000000000002</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>21.2</v>
       </c>
@@ -3584,7 +3553,7 @@
         <v>2.0779999999999998</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>23.2</v>
       </c>
@@ -3610,7 +3579,7 @@
         <v>2.0329999999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>25.1</v>
       </c>
@@ -3636,7 +3605,7 @@
         <v>1.976</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>27</v>
       </c>
@@ -3662,7 +3631,7 @@
         <v>1.907</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>29</v>
       </c>
@@ -3688,7 +3657,7 @@
         <v>1.8260000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>30.9</v>
       </c>
@@ -3714,7 +3683,7 @@
         <v>1.734</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>32.799999999999997</v>
       </c>
@@ -3740,7 +3709,7 @@
         <v>1.629</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>34.799999999999997</v>
       </c>
@@ -3766,7 +3735,7 @@
         <v>1.512</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>36.700000000000003</v>
       </c>
@@ -3792,7 +3761,7 @@
         <v>1.387</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>38.6</v>
       </c>
@@ -3818,7 +3787,7 @@
         <v>1.258</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>40.6</v>
       </c>
@@ -3844,7 +3813,7 @@
         <v>1.127</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>42.5</v>
       </c>
@@ -3870,7 +3839,7 @@
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>44.4</v>
       </c>
@@ -3896,7 +3865,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>46.3</v>
       </c>
@@ -3922,7 +3891,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>48.3</v>
       </c>
@@ -3948,7 +3917,7 @@
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>50.2</v>
       </c>
@@ -3974,7 +3943,7 @@
         <v>0.434</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>52.1</v>
       </c>
@@ -4000,7 +3969,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>54.1</v>
       </c>
@@ -4026,7 +3995,7 @@
         <v>0.14599999999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>56</v>
       </c>
@@ -4052,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>30</v>
       </c>
@@ -4066,7 +4035,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>26</v>
       </c>
@@ -4092,7 +4061,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>40</v>
       </c>
@@ -4112,7 +4081,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>0</v>
       </c>
@@ -4138,7 +4107,7 @@
         <v>3.4590000000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2.4</v>
       </c>
@@ -4164,7 +4133,7 @@
         <v>3.4630000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>4.8</v>
       </c>
@@ -4190,7 +4159,7 @@
         <v>3.4660000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>7.2</v>
       </c>
@@ -4216,7 +4185,7 @@
         <v>3.468</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>9.6</v>
       </c>
@@ -4242,7 +4211,7 @@
         <v>3.4689999999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>12</v>
       </c>
@@ -4268,7 +4237,7 @@
         <v>3.4670000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>14.5</v>
       </c>
@@ -4294,7 +4263,7 @@
         <v>3.4630000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>16.899999999999999</v>
       </c>
@@ -4320,7 +4289,7 @@
         <v>3.4550000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>19.3</v>
       </c>
@@ -4346,7 +4315,7 @@
         <v>3.4409999999999998</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>21.7</v>
       </c>
@@ -4372,7 +4341,7 @@
         <v>3.4169999999999998</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>24.1</v>
       </c>
@@ -4398,7 +4367,7 @@
         <v>3.3759999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>26.5</v>
       </c>
@@ -4424,7 +4393,7 @@
         <v>3.3180000000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>28.9</v>
       </c>
@@ -4450,7 +4419,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>31.3</v>
       </c>
@@ -4476,7 +4445,7 @@
         <v>3.1429999999999998</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>33.700000000000003</v>
       </c>
@@ -4502,7 +4471,7 @@
         <v>3.0270000000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>36.1</v>
       </c>
@@ -4528,7 +4497,7 @@
         <v>2.8929999999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>38.5</v>
       </c>
@@ -4554,7 +4523,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>41</v>
       </c>
@@ -4580,7 +4549,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>43.4</v>
       </c>
@@ -4606,7 +4575,7 @@
         <v>2.383</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>45.8</v>
       </c>
@@ -4632,7 +4601,7 @@
         <v>2.1850000000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>48.2</v>
       </c>
@@ -4658,7 +4627,7 @@
         <v>1.9850000000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>50.6</v>
       </c>
@@ -4684,7 +4653,7 @@
         <v>1.7789999999999999</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>53</v>
       </c>
@@ -4710,7 +4679,7 @@
         <v>1.569</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>55.4</v>
       </c>
@@ -4736,7 +4705,7 @@
         <v>1.355</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>57.8</v>
       </c>
@@ -4762,7 +4731,7 @@
         <v>1.1379999999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>60.2</v>
       </c>
@@ -4788,7 +4757,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>62.6</v>
       </c>
@@ -4814,7 +4783,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>65</v>
       </c>
@@ -4840,7 +4809,7 @@
         <v>0.46300000000000002</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>67.5</v>
       </c>
@@ -4866,7 +4835,7 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>69.900000000000006</v>
       </c>
@@ -4892,7 +4861,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>30</v>
       </c>
@@ -4906,7 +4875,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>26</v>
       </c>
@@ -4932,7 +4901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>40</v>
       </c>
@@ -4952,7 +4921,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>0</v>
       </c>
@@ -4978,7 +4947,7 @@
         <v>5.1509999999999998</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>2.9</v>
       </c>
@@ -5004,7 +4973,7 @@
         <v>5.1580000000000004</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>5.8</v>
       </c>
@@ -5030,7 +4999,7 @@
         <v>5.1630000000000003</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>8.6999999999999993</v>
       </c>
@@ -5056,7 +5025,7 @@
         <v>5.1660000000000004</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>11.6</v>
       </c>
@@ -5082,7 +5051,7 @@
         <v>5.165</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>14.4</v>
       </c>
@@ -5108,7 +5077,7 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>17.3</v>
       </c>
@@ -5134,7 +5103,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>20.2</v>
       </c>
@@ -5160,7 +5129,7 @@
         <v>5.1319999999999997</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>23.1</v>
       </c>
@@ -5186,7 +5155,7 @@
         <v>5.1040000000000001</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>26</v>
       </c>
@@ -5212,7 +5181,7 @@
         <v>5.0609999999999999</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>28.9</v>
       </c>
@@ -5238,7 +5207,7 @@
         <v>4.9939999999999998</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>31.8</v>
       </c>
@@ -5264,7 +5233,7 @@
         <v>4.8970000000000002</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>34.700000000000003</v>
       </c>
@@ -5290,7 +5259,7 @@
         <v>4.7720000000000002</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>37.6</v>
       </c>
@@ -5316,7 +5285,7 @@
         <v>4.6180000000000003</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>40.5</v>
       </c>
@@ -5342,7 +5311,7 @@
         <v>4.4359999999999999</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>43.3</v>
       </c>
@@ -5368,7 +5337,7 @@
         <v>4.2270000000000003</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>46.2</v>
       </c>
@@ -5394,7 +5363,7 @@
         <v>3.9940000000000002</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>49.1</v>
       </c>
@@ -5420,7 +5389,7 @@
         <v>3.738</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>52</v>
       </c>
@@ -5446,7 +5415,7 @@
         <v>3.4609999999999999</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>54.9</v>
       </c>
@@ -5472,7 +5441,7 @@
         <v>3.1709999999999998</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>57.8</v>
       </c>
@@ -5498,7 +5467,7 @@
         <v>2.879</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>60.7</v>
       </c>
@@ -5524,7 +5493,7 @@
         <v>2.581</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>63.6</v>
       </c>
@@ -5550,7 +5519,7 @@
         <v>2.2770000000000001</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>66.5</v>
       </c>
@@ -5576,7 +5545,7 @@
         <v>1.968</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>69.400000000000006</v>
       </c>
@@ -5602,7 +5571,7 @@
         <v>1.6539999999999999</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>72.2</v>
       </c>
@@ -5628,7 +5597,7 @@
         <v>1.3340000000000001</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>75.099999999999994</v>
       </c>
@@ -5654,7 +5623,7 @@
         <v>1.0089999999999999</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>78</v>
       </c>
@@ -5680,7 +5649,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>80.900000000000006</v>
       </c>
@@ -5706,7 +5675,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>83.8</v>
       </c>
@@ -5732,7 +5701,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>30</v>
       </c>
@@ -5746,7 +5715,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>26</v>
       </c>
@@ -5772,7 +5741,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>40</v>
       </c>
@@ -5792,7 +5761,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>0</v>
       </c>
@@ -5818,7 +5787,7 @@
         <v>7.2190000000000003</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>3.4</v>
       </c>
@@ -5844,7 +5813,7 @@
         <v>7.2309999999999999</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>6.8</v>
       </c>
@@ -5870,7 +5839,7 @@
         <v>7.2389999999999999</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>10.1</v>
       </c>
@@ -5896,7 +5865,7 @@
         <v>7.242</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>13.5</v>
       </c>
@@ -5922,7 +5891,7 @@
         <v>7.2389999999999999</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>16.899999999999999</v>
       </c>
@@ -5948,7 +5917,7 @@
         <v>7.2290000000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>20.3</v>
       </c>
@@ -5974,7 +5943,7 @@
         <v>7.21</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>23.6</v>
       </c>
@@ -6000,7 +5969,7 @@
         <v>7.1790000000000003</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>27</v>
       </c>
@@ -6026,7 +5995,7 @@
         <v>7.133</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>30.4</v>
       </c>
@@ -6052,7 +6021,7 @@
         <v>7.0670000000000002</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>33.799999999999997</v>
       </c>
@@ -6078,7 +6047,7 @@
         <v>6.9690000000000003</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>37.1</v>
       </c>
@@ -6104,7 +6073,7 @@
         <v>6.8250000000000002</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>40.5</v>
       </c>
@@ -6130,7 +6099,7 @@
         <v>6.6369999999999996</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>43.9</v>
       </c>
@@ -6156,7 +6125,7 @@
         <v>6.4089999999999998</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>47.3</v>
       </c>
@@ -6182,7 +6151,7 @@
         <v>6.141</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>50.6</v>
       </c>
@@ -6208,7 +6177,7 @@
         <v>5.8369999999999997</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>54</v>
       </c>
@@ -6234,7 +6203,7 @@
         <v>5.5019999999999998</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>57.4</v>
       </c>
@@ -6260,7 +6229,7 @@
         <v>5.1390000000000002</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>60.8</v>
       </c>
@@ -6286,7 +6255,7 @@
         <v>4.7510000000000003</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>64.099999999999994</v>
       </c>
@@ -6312,7 +6281,7 @@
         <v>4.3499999999999996</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>67.5</v>
       </c>
@@ -6338,7 +6307,7 @@
         <v>3.948</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>70.900000000000006</v>
       </c>
@@ -6364,7 +6333,7 @@
         <v>3.5379999999999998</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>74.3</v>
       </c>
@@ -6390,7 +6359,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>77.599999999999994</v>
       </c>
@@ -6416,7 +6385,7 @@
         <v>2.6930000000000001</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>81</v>
       </c>
@@ -6442,7 +6411,7 @@
         <v>2.2589999999999999</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>84.4</v>
       </c>
@@ -6468,7 +6437,7 @@
         <v>1.8160000000000001</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>87.8</v>
       </c>
@@ -6494,7 +6463,7 @@
         <v>1.3640000000000001</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>91.1</v>
       </c>
@@ -6520,7 +6489,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>94.5</v>
       </c>
@@ -6546,7 +6515,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>97.9</v>
       </c>
@@ -6572,7 +6541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>30</v>
       </c>
@@ -6586,7 +6555,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>26</v>
       </c>
@@ -6612,7 +6581,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>40</v>
       </c>
@@ -6632,7 +6601,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>0</v>
       </c>
@@ -6658,7 +6627,7 @@
         <v>9.6820000000000004</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>3.9</v>
       </c>
@@ -6684,7 +6653,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>7.7</v>
       </c>
@@ -6710,7 +6679,7 @@
         <v>9.7129999999999992</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>11.6</v>
       </c>
@@ -6736,7 +6705,7 @@
         <v>9.7170000000000005</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>15.4</v>
       </c>
@@ -6762,7 +6731,7 @@
         <v>9.7119999999999997</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>19.3</v>
       </c>
@@ -6788,7 +6757,7 @@
         <v>9.6959999999999997</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>23.1</v>
       </c>
@@ -6814,7 +6783,7 @@
         <v>9.6660000000000004</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>27</v>
       </c>
@@ -6840,7 +6809,7 @@
         <v>9.6189999999999998</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>30.8</v>
       </c>
@@ -6866,7 +6835,7 @@
         <v>9.5510000000000002</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>34.700000000000003</v>
       </c>
@@ -6892,7 +6861,7 @@
         <v>9.4559999999999995</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>38.5</v>
       </c>
@@ -6918,7 +6887,7 @@
         <v>9.3249999999999993</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>42.4</v>
       </c>
@@ -6944,7 +6913,7 @@
         <v>9.1310000000000002</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>46.2</v>
       </c>
@@ -6970,7 +6939,7 @@
         <v>8.8699999999999992</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>50.1</v>
       </c>
@@ -6996,7 +6965,7 @@
         <v>8.5519999999999996</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>53.9</v>
       </c>
@@ -7022,7 +6991,7 @@
         <v>8.18</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>57.8</v>
       </c>
@@ -7048,7 +7017,7 @@
         <v>7.7610000000000001</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>61.6</v>
       </c>
@@ -7074,7 +7043,7 @@
         <v>7.3029999999999999</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>65.5</v>
       </c>
@@ -7100,7 +7069,7 @@
         <v>6.8120000000000003</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>69.3</v>
       </c>
@@ -7126,7 +7095,7 @@
         <v>6.2930000000000001</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>73.2</v>
       </c>
@@ -7152,7 +7121,7 @@
         <v>5.7619999999999996</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>77.099999999999994</v>
       </c>
@@ -7178,7 +7147,7 @@
         <v>5.2329999999999997</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>80.900000000000006</v>
       </c>
@@ -7204,7 +7173,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>84.8</v>
       </c>
@@ -7230,7 +7199,7 @@
         <v>4.1369999999999996</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>88.6</v>
       </c>
@@ -7256,7 +7225,7 @@
         <v>3.5739999999999998</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>92.5</v>
       </c>
@@ -7282,7 +7251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>96.3</v>
       </c>
@@ -7308,7 +7277,7 @@
         <v>2.4159999999999999</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>100.2</v>
       </c>
@@ -7334,7 +7303,7 @@
         <v>1.8240000000000001</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>104</v>
       </c>
@@ -7360,7 +7329,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>107.9</v>
       </c>
@@ -7386,7 +7355,7 @@
         <v>0.61499999999999999</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>111.7</v>
       </c>
@@ -7412,7 +7381,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>30</v>
       </c>
@@ -7426,7 +7395,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>26</v>
       </c>
@@ -7452,7 +7421,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>40</v>
       </c>
@@ -7472,7 +7441,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>0</v>
       </c>
@@ -7498,7 +7467,7 @@
         <v>12.211</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>4.3</v>
       </c>
@@ -7524,7 +7493,7 @@
         <v>12.234</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>8.6999999999999993</v>
       </c>
@@ -7550,7 +7519,7 @@
         <v>12.247999999999999</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>13</v>
       </c>
@@ -7576,7 +7545,7 @@
         <v>12.254</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>17.3</v>
       </c>
@@ -7602,7 +7571,7 @@
         <v>12.247</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>21.7</v>
       </c>
@@ -7628,7 +7597,7 @@
         <v>12.224</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>26</v>
       </c>
@@ -7654,7 +7623,7 @@
         <v>12.186</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>30.3</v>
       </c>
@@ -7680,7 +7649,7 @@
         <v>12.129</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>34.700000000000003</v>
       </c>
@@ -7706,7 +7675,7 @@
         <v>12.048</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>39</v>
       </c>
@@ -7732,7 +7701,7 @@
         <v>11.94</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>43.3</v>
       </c>
@@ -7758,7 +7727,7 @@
         <v>11.792999999999999</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>47.7</v>
       </c>
@@ -7784,7 +7753,7 @@
         <v>11.584</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>52</v>
       </c>
@@ -7810,7 +7779,7 @@
         <v>11.28</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>56.3</v>
       </c>
@@ -7836,7 +7805,7 @@
         <v>10.894</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>60.7</v>
       </c>
@@ -7862,7 +7831,7 @@
         <v>10.438000000000001</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>65</v>
       </c>
@@ -7888,7 +7857,7 @@
         <v>9.9190000000000005</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>69.3</v>
       </c>
@@ -7914,7 +7883,7 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>73.7</v>
       </c>
@@ -7940,7 +7909,7 @@
         <v>8.734</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>78</v>
       </c>
@@ -7966,7 +7935,7 @@
         <v>8.0809999999999995</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>82.3</v>
       </c>
@@ -7992,7 +7961,7 @@
         <v>7.4029999999999996</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>86.7</v>
       </c>
@@ -8018,7 +7987,7 @@
         <v>6.7240000000000002</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>91</v>
       </c>
@@ -8044,7 +8013,7 @@
         <v>6.0289999999999999</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>95.3</v>
       </c>
@@ -8070,7 +8039,7 @@
         <v>5.3220000000000001</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>99.7</v>
       </c>
@@ -8096,7 +8065,7 @@
         <v>4.601</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>104</v>
       </c>
@@ -8122,7 +8091,7 @@
         <v>3.8639999999999999</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>108.3</v>
       </c>
@@ -8148,7 +8117,7 @@
         <v>3.113</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>112.7</v>
       </c>
@@ -8174,7 +8143,7 @@
         <v>2.3519999999999999</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>117</v>
       </c>
@@ -8200,7 +8169,7 @@
         <v>1.5820000000000001</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>121.3</v>
       </c>
@@ -8226,7 +8195,7 @@
         <v>0.79500000000000004</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>125.7</v>
       </c>
@@ -8252,7 +8221,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>30</v>
       </c>
@@ -8266,7 +8235,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>26</v>
       </c>
@@ -8292,7 +8261,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>40</v>
       </c>
@@ -8312,7 +8281,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>0</v>
       </c>
@@ -8338,7 +8307,7 @@
         <v>14.605</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>4.8</v>
       </c>
@@ -8364,7 +8333,7 @@
         <v>14.629</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>9.6</v>
       </c>
@@ -8390,7 +8359,7 @@
         <v>14.648</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>14.4</v>
       </c>
@@ -8416,7 +8385,7 @@
         <v>14.657</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>19.3</v>
       </c>
@@ -8442,7 +8411,7 @@
         <v>14.657999999999999</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>24.1</v>
       </c>
@@ -8468,7 +8437,7 @@
         <v>14.647</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>28.9</v>
       </c>
@@ -8494,7 +8463,7 @@
         <v>14.622</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>33.700000000000003</v>
       </c>
@@ -8520,7 +8489,7 @@
         <v>14.58</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>38.5</v>
       </c>
@@ -8546,7 +8515,7 @@
         <v>14.519</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>43.3</v>
       </c>
@@ -8572,7 +8541,7 @@
         <v>14.433999999999999</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>48.1</v>
       </c>
@@ -8598,7 +8567,7 @@
         <v>14.317</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>53</v>
       </c>
@@ -8624,7 +8593,7 @@
         <v>14.151</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>57.8</v>
       </c>
@@ -8650,7 +8619,7 @@
         <v>13.872999999999999</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>62.6</v>
       </c>
@@ -8676,7 +8645,7 @@
         <v>13.465999999999999</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>67.400000000000006</v>
       </c>
@@ -8702,7 +8671,7 @@
         <v>12.957000000000001</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>72.2</v>
       </c>
@@ -8728,7 +8697,7 @@
         <v>12.36</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>77</v>
       </c>
@@ -8754,7 +8723,7 @@
         <v>11.689</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>81.900000000000006</v>
       </c>
@@ -8780,7 +8749,7 @@
         <v>10.951000000000001</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>86.7</v>
       </c>
@@ -8806,7 +8775,7 @@
         <v>10.153</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>91.5</v>
       </c>
@@ -8832,7 +8801,7 @@
         <v>9.3059999999999992</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>96.3</v>
       </c>
@@ -8858,7 +8827,7 @@
         <v>8.452</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>101.1</v>
       </c>
@@ -8884,7 +8853,7 @@
         <v>7.5819999999999999</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>105.9</v>
       </c>
@@ -8910,7 +8879,7 @@
         <v>6.6929999999999996</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>110.7</v>
       </c>
@@ -8936,7 +8905,7 @@
         <v>5.7859999999999996</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>115.6</v>
       </c>
@@ -8962,7 +8931,7 @@
         <v>4.859</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>120.4</v>
       </c>
@@ -8988,7 +8957,7 @@
         <v>3.9180000000000001</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>125.2</v>
       </c>
@@ -9014,7 +8983,7 @@
         <v>2.9630000000000001</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>130</v>
       </c>
@@ -9040,7 +9009,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>134.80000000000001</v>
       </c>
@@ -9066,7 +9035,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>139.6</v>
       </c>
@@ -9092,7 +9061,7 @@
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>30</v>
       </c>
@@ -9106,7 +9075,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>26</v>
       </c>
@@ -9132,7 +9101,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>40</v>
       </c>
@@ -9152,7 +9121,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>0</v>
       </c>
@@ -9178,7 +9147,7 @@
         <v>17.126000000000001</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>5.3</v>
       </c>
@@ -9204,7 +9173,7 @@
         <v>17.151</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>10.6</v>
       </c>
@@ -9230,7 +9199,7 @@
         <v>17.172000000000001</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>15.9</v>
       </c>
@@ -9256,7 +9225,7 @@
         <v>17.187000000000001</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>21.2</v>
       </c>
@@ -9282,7 +9251,7 @@
         <v>17.196000000000002</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>26.5</v>
       </c>
@@ -9308,7 +9277,7 @@
         <v>17.199000000000002</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>31.7</v>
       </c>
@@ -9334,7 +9303,7 @@
         <v>17.193000000000001</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>37</v>
       </c>
@@ -9360,7 +9329,7 @@
         <v>17.175000000000001</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>42.3</v>
       </c>
@@ -9386,7 +9355,7 @@
         <v>17.143999999999998</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>47.6</v>
       </c>
@@ -9412,7 +9381,7 @@
         <v>17.096</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>52.9</v>
       </c>
@@ -9438,7 +9407,7 @@
         <v>17.026</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>58.2</v>
       </c>
@@ -9464,7 +9433,7 @@
         <v>16.920999999999999</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>63.5</v>
       </c>
@@ -9490,7 +9459,7 @@
         <v>16.748000000000001</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>68.8</v>
       </c>
@@ -9516,7 +9485,7 @@
         <v>16.379000000000001</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>74.099999999999994</v>
       </c>
@@ -9542,7 +9511,7 @@
         <v>15.842000000000001</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>79.400000000000006</v>
       </c>
@@ -9568,7 +9537,7 @@
         <v>15.176</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>84.7</v>
       </c>
@@ -9594,7 +9563,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>90</v>
       </c>
@@ -9620,7 +9589,7 @@
         <v>13.53</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>95.2</v>
       </c>
@@ -9646,7 +9615,7 @@
         <v>12.574</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>100.5</v>
       </c>
@@ -9672,7 +9641,7 @@
         <v>11.538</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>105.8</v>
       </c>
@@ -9698,7 +9667,7 @@
         <v>10.484</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>111.1</v>
       </c>
@@ -9724,7 +9693,7 @@
         <v>9.4149999999999991</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>116.4</v>
       </c>
@@ -9750,7 +9719,7 @@
         <v>8.3239999999999998</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>121.7</v>
       </c>
@@ -9776,7 +9745,7 @@
         <v>7.2039999999999997</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>127</v>
       </c>
@@ -9802,7 +9771,7 @@
         <v>6.0510000000000002</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>132.30000000000001</v>
       </c>
@@ -9828,7 +9797,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>137.6</v>
       </c>
@@ -9854,7 +9823,7 @@
         <v>3.7170000000000001</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>142.9</v>
       </c>
@@ -9880,7 +9849,7 @@
         <v>2.5049999999999999</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>148.19999999999999</v>
       </c>
@@ -9906,7 +9875,7 @@
         <v>1.2609999999999999</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>153.4</v>
       </c>
@@ -9932,7 +9901,7 @@
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>30</v>
       </c>
@@ -9946,7 +9915,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>26</v>
       </c>
@@ -9972,7 +9941,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>40</v>
       </c>
@@ -9992,7 +9961,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>0</v>
       </c>
@@ -10018,7 +9987,7 @@
         <v>19.741</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>5.8</v>
       </c>
@@ -10044,7 +10013,7 @@
         <v>19.765000000000001</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>11.5</v>
       </c>
@@ -10070,7 +10039,7 @@
         <v>19.786999999999999</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>17.3</v>
       </c>
@@ -10096,7 +10065,7 @@
         <v>19.808</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>23.1</v>
       </c>
@@ -10122,7 +10091,7 @@
         <v>19.826000000000001</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>28.8</v>
       </c>
@@ -10148,7 +10117,7 @@
         <v>19.841999999999999</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>34.6</v>
       </c>
@@ -10174,7 +10143,7 @@
         <v>19.856000000000002</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>40.4</v>
       </c>
@@ -10200,7 +10169,7 @@
         <v>19.867999999999999</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>46.1</v>
       </c>
@@ -10226,7 +10195,7 @@
         <v>19.878</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>51.9</v>
       </c>
@@ -10252,7 +10221,7 @@
         <v>19.888000000000002</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>57.7</v>
       </c>
@@ -10278,7 +10247,7 @@
         <v>19.887</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>63.4</v>
       </c>
@@ -10304,7 +10273,7 @@
         <v>19.873999999999999</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>69.2</v>
       </c>
@@ -10330,7 +10299,7 @@
         <v>19.831</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>74.900000000000006</v>
       </c>
@@ -10356,7 +10325,7 @@
         <v>19.684999999999999</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>80.7</v>
       </c>
@@ -10382,7 +10351,7 @@
         <v>19.173999999999999</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>86.5</v>
       </c>
@@ -10408,7 +10377,7 @@
         <v>18.454000000000001</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>92.2</v>
       </c>
@@ -10434,7 +10403,7 @@
         <v>17.576000000000001</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>98</v>
       </c>
@@ -10460,7 +10429,7 @@
         <v>16.559000000000001</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>103.8</v>
       </c>
@@ -10486,7 +10455,7 @@
         <v>15.423999999999999</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>109.5</v>
       </c>
@@ -10512,7 +10481,7 @@
         <v>14.175000000000001</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>115.3</v>
       </c>
@@ -10538,7 +10507,7 @@
         <v>12.895</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>121.1</v>
       </c>
@@ -10564,7 +10533,7 @@
         <v>11.587</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>126.8</v>
       </c>
@@ -10590,7 +10559,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="448" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>132.6</v>
       </c>
@@ -10616,7 +10585,7 @@
         <v>8.8800000000000008</v>
       </c>
     </row>
-    <row r="449" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>138.4</v>
       </c>
@@ -10642,7 +10611,7 @@
         <v>7.4779999999999998</v>
       </c>
     </row>
-    <row r="450" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>144.1</v>
       </c>
@@ -10668,7 +10637,7 @@
         <v>6.0510000000000002</v>
       </c>
     </row>
-    <row r="451" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>149.9</v>
       </c>
@@ -10694,7 +10663,7 @@
         <v>4.5919999999999996</v>
       </c>
     </row>
-    <row r="452" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>155.69999999999999</v>
       </c>
@@ -10720,7 +10689,7 @@
         <v>3.1120000000000001</v>
       </c>
     </row>
-    <row r="453" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>161.4</v>
       </c>
@@ -10746,7 +10715,7 @@
         <v>1.5640000000000001</v>
       </c>
     </row>
-    <row r="454" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>167.2</v>
       </c>
@@ -10772,7 +10741,7 @@
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="458" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>30</v>
       </c>
@@ -10786,7 +10755,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="460" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>26</v>
       </c>
@@ -10812,7 +10781,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="461" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>40</v>
       </c>
@@ -10832,7 +10801,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="462" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>0</v>
       </c>
@@ -10858,7 +10827,7 @@
         <v>22.917999999999999</v>
       </c>
     </row>
-    <row r="463" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>6.2</v>
       </c>
@@ -10884,7 +10853,7 @@
         <v>22.943000000000001</v>
       </c>
     </row>
-    <row r="464" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>12.5</v>
       </c>
@@ -10910,7 +10879,7 @@
         <v>22.957000000000001</v>
       </c>
     </row>
-    <row r="465" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>18.7</v>
       </c>
@@ -10936,7 +10905,7 @@
         <v>22.997</v>
       </c>
     </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>25</v>
       </c>
@@ -10962,7 +10931,7 @@
         <v>23.027000000000001</v>
       </c>
     </row>
-    <row r="467" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>31.2</v>
       </c>
@@ -10988,7 +10957,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="468" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>37.5</v>
       </c>
@@ -11014,7 +10983,7 @@
         <v>23.091999999999999</v>
       </c>
     </row>
-    <row r="469" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>43.7</v>
       </c>
@@ -11040,7 +11009,7 @@
         <v>23.128</v>
       </c>
     </row>
-    <row r="470" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>50</v>
       </c>
@@ -11066,7 +11035,7 @@
         <v>23.169</v>
       </c>
     </row>
-    <row r="471" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>56.2</v>
       </c>
@@ -11092,7 +11061,7 @@
         <v>23.21</v>
       </c>
     </row>
-    <row r="472" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>62.5</v>
       </c>
@@ -11118,7 +11087,7 @@
         <v>23.254999999999999</v>
       </c>
     </row>
-    <row r="473" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>68.7</v>
       </c>
@@ -11144,7 +11113,7 @@
         <v>23.297000000000001</v>
       </c>
     </row>
-    <row r="474" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>74.900000000000006</v>
       </c>
@@ -11170,7 +11139,7 @@
         <v>23.361999999999998</v>
       </c>
     </row>
-    <row r="475" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>81.2</v>
       </c>
@@ -11196,7 +11165,7 @@
         <v>23.416</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>87.4</v>
       </c>
@@ -11222,7 +11191,7 @@
         <v>23.434999999999999</v>
       </c>
     </row>
-    <row r="477" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>93.7</v>
       </c>
@@ -11248,7 +11217,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="478" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>99.9</v>
       </c>
@@ -11274,7 +11243,7 @@
         <v>21.901</v>
       </c>
     </row>
-    <row r="479" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>106.2</v>
       </c>
@@ -11300,7 +11269,7 @@
         <v>20.593</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>112.4</v>
       </c>
@@ -11326,7 +11295,7 @@
         <v>19.148</v>
       </c>
     </row>
-    <row r="481" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>118.7</v>
       </c>
@@ -11352,7 +11321,7 @@
         <v>17.527999999999999</v>
       </c>
     </row>
-    <row r="482" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>124.9</v>
       </c>
@@ -11378,7 +11347,7 @@
         <v>15.919</v>
       </c>
     </row>
-    <row r="483" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>131.19999999999999</v>
       </c>
@@ -11404,7 +11373,7 @@
         <v>14.275</v>
       </c>
     </row>
-    <row r="484" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>137.4</v>
       </c>
@@ -11430,7 +11399,7 @@
         <v>12.597</v>
       </c>
     </row>
-    <row r="485" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>143.6</v>
       </c>
@@ -11456,7 +11425,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="486" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>149.9</v>
       </c>
@@ -11482,7 +11451,7 @@
         <v>9.1690000000000005</v>
       </c>
     </row>
-    <row r="487" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A487">
         <v>156.1</v>
       </c>
@@ -11508,7 +11477,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="488" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A488">
         <v>162.4</v>
       </c>
@@ -11534,7 +11503,7 @@
         <v>5.6109999999999998</v>
       </c>
     </row>
-    <row r="489" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>168.6</v>
       </c>
@@ -11560,7 +11529,7 @@
         <v>3.754</v>
       </c>
     </row>
-    <row r="490" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>174.9</v>
       </c>
@@ -11586,7 +11555,7 @@
         <v>1.9239999999999999</v>
       </c>
     </row>
-    <row r="491" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>181.1</v>
       </c>
@@ -11612,7 +11581,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="495" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>30</v>
       </c>
@@ -11626,7 +11595,7 @@
         <v>13999</v>
       </c>
     </row>
-    <row r="497" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>26</v>
       </c>
@@ -11652,7 +11621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="498" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>40</v>
       </c>
@@ -11672,7 +11641,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="499" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A499">
         <v>0</v>
       </c>
@@ -11698,7 +11667,7 @@
         <v>26.829000000000001</v>
       </c>
     </row>
-    <row r="500" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A500">
         <v>6.7</v>
       </c>
@@ -11724,7 +11693,7 @@
         <v>26.866</v>
       </c>
     </row>
-    <row r="501" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A501">
         <v>13.4</v>
       </c>
@@ -11750,7 +11719,7 @@
         <v>26.908000000000001</v>
       </c>
     </row>
-    <row r="502" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>20.100000000000001</v>
       </c>
@@ -11776,7 +11745,7 @@
         <v>26.960999999999999</v>
       </c>
     </row>
-    <row r="503" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A503">
         <v>26.8</v>
       </c>
@@ -11802,7 +11771,7 @@
         <v>26.818999999999999</v>
       </c>
     </row>
-    <row r="504" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A504">
         <v>33.5</v>
       </c>
@@ -11828,7 +11797,7 @@
         <v>26.885000000000002</v>
       </c>
     </row>
-    <row r="505" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A505">
         <v>40.1</v>
       </c>
@@ -11854,7 +11823,7 @@
         <v>27.038</v>
       </c>
     </row>
-    <row r="506" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A506">
         <v>46.8</v>
       </c>
@@ -11880,7 +11849,7 @@
         <v>27.338000000000001</v>
       </c>
     </row>
-    <row r="507" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A507">
         <v>53.5</v>
       </c>
@@ -11906,7 +11875,7 @@
         <v>27.173999999999999</v>
       </c>
     </row>
-    <row r="508" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A508">
         <v>60.2</v>
       </c>
@@ -11932,7 +11901,7 @@
         <v>27.414000000000001</v>
       </c>
     </row>
-    <row r="509" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A509">
         <v>66.900000000000006</v>
       </c>
@@ -11958,7 +11927,7 @@
         <v>27.44</v>
       </c>
     </row>
-    <row r="510" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A510">
         <v>73.599999999999994</v>
       </c>
@@ -11984,7 +11953,7 @@
         <v>27.443000000000001</v>
       </c>
     </row>
-    <row r="511" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>80.3</v>
       </c>
@@ -12010,7 +11979,7 @@
         <v>27.440999999999999</v>
       </c>
     </row>
-    <row r="512" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A512">
         <v>87</v>
       </c>
@@ -12036,7 +12005,7 @@
         <v>27.335000000000001</v>
       </c>
     </row>
-    <row r="513" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A513">
         <v>93.7</v>
       </c>
@@ -12062,7 +12031,7 @@
         <v>27.413</v>
       </c>
     </row>
-    <row r="514" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A514">
         <v>100.4</v>
       </c>
@@ -12088,7 +12057,7 @@
         <v>27.353999999999999</v>
       </c>
     </row>
-    <row r="515" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A515">
         <v>107</v>
       </c>
@@ -12114,7 +12083,7 @@
         <v>26.773</v>
       </c>
     </row>
-    <row r="516" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A516">
         <v>113.7</v>
       </c>
@@ -12140,7 +12109,7 @@
         <v>25.763000000000002</v>
       </c>
     </row>
-    <row r="517" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A517">
         <v>120.4</v>
       </c>
@@ -12166,7 +12135,7 @@
         <v>24.425000000000001</v>
       </c>
     </row>
-    <row r="518" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A518">
         <v>127.1</v>
       </c>
@@ -12192,7 +12161,7 @@
         <v>22.763000000000002</v>
       </c>
     </row>
-    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A519">
         <v>133.80000000000001</v>
       </c>
@@ -12218,7 +12187,7 @@
         <v>20.715</v>
       </c>
     </row>
-    <row r="520" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A520">
         <v>140.5</v>
       </c>
@@ -12244,7 +12213,7 @@
         <v>18.629000000000001</v>
       </c>
     </row>
-    <row r="521" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A521">
         <v>147.19999999999999</v>
       </c>
@@ -12270,7 +12239,7 @@
         <v>16.509</v>
       </c>
     </row>
-    <row r="522" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A522">
         <v>153.9</v>
       </c>
@@ -12296,63 +12265,59 @@
         <v>14.461</v>
       </c>
     </row>
-    <row r="523" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A523">
         <v>160.6</v>
       </c>
-      <c r="B523" t="s">
-        <v>46</v>
-      </c>
-      <c r="C523" t="e" cm="1">
-        <f t="array" ref="C523">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D523" t="e" cm="1">
-        <f t="array" ref="D523">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E523" t="e" cm="1">
-        <f t="array" ref="E523">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F523" t="e" cm="1">
-        <f t="array" ref="F523">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G523" t="e" cm="1">
-        <f t="array" ref="G523">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="524" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B523">
+        <v>0.87</v>
+      </c>
+      <c r="C523">
+        <v>0</v>
+      </c>
+      <c r="D523">
+        <v>0</v>
+      </c>
+      <c r="E523">
+        <v>0</v>
+      </c>
+      <c r="F523">
+        <v>0</v>
+      </c>
+      <c r="G523">
+        <v>0</v>
+      </c>
+      <c r="H523">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A524">
         <v>167.3</v>
       </c>
-      <c r="B524" t="s">
-        <v>47</v>
-      </c>
-      <c r="C524" t="e" cm="1">
-        <f t="array" ref="C524">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D524" t="e" cm="1">
-        <f t="array" ref="D524">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E524" t="e" cm="1">
-        <f t="array" ref="E524">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F524" t="e" cm="1">
-        <f t="array" ref="F524">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G524" t="e" cm="1">
-        <f t="array" ref="G524">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B524">
+        <v>0.9</v>
+      </c>
+      <c r="C524">
+        <v>0</v>
+      </c>
+      <c r="D524">
+        <v>0</v>
+      </c>
+      <c r="E524">
+        <v>0</v>
+      </c>
+      <c r="F524">
+        <v>0</v>
+      </c>
+      <c r="G524">
+        <v>0</v>
+      </c>
+      <c r="H524">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A525">
         <v>174</v>
       </c>
@@ -12378,7 +12343,7 @@
         <v>7.3150000000000004</v>
       </c>
     </row>
-    <row r="526" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A526">
         <v>180.6</v>
       </c>
@@ -12404,7 +12369,7 @@
         <v>4.9329999999999998</v>
       </c>
     </row>
-    <row r="527" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A527">
         <v>187.3</v>
       </c>
@@ -12430,7 +12395,7 @@
         <v>2.6269999999999998</v>
       </c>
     </row>
-    <row r="528" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A528">
         <v>194</v>
       </c>
@@ -12456,7 +12421,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>30</v>
       </c>
@@ -12470,7 +12435,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="534" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>26</v>
       </c>
@@ -12496,7 +12461,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="535" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>40</v>
       </c>
@@ -12516,7 +12481,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="536" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A536">
         <v>0</v>
       </c>
@@ -12542,7 +12507,7 @@
         <v>35.406999999999996</v>
       </c>
     </row>
-    <row r="537" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A537">
         <v>7.7</v>
       </c>
@@ -12568,7 +12533,7 @@
         <v>35.469000000000001</v>
       </c>
     </row>
-    <row r="538" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A538">
         <v>15.4</v>
       </c>
@@ -12594,7 +12559,7 @@
         <v>35.529000000000003</v>
       </c>
     </row>
-    <row r="539" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A539">
         <v>23</v>
       </c>
@@ -12620,7 +12585,7 @@
         <v>35.097000000000001</v>
       </c>
     </row>
-    <row r="540" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A540">
         <v>30.7</v>
       </c>
@@ -12646,7 +12611,7 @@
         <v>35.128</v>
       </c>
     </row>
-    <row r="541" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A541">
         <v>38.4</v>
       </c>
@@ -12672,7 +12637,7 @@
         <v>35.603999999999999</v>
       </c>
     </row>
-    <row r="542" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A542">
         <v>46.1</v>
       </c>
@@ -12698,7 +12663,7 @@
         <v>35.594000000000001</v>
       </c>
     </row>
-    <row r="543" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A543">
         <v>53.7</v>
       </c>
@@ -12724,7 +12689,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="544" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A544">
         <v>61.4</v>
       </c>
@@ -12750,7 +12715,7 @@
         <v>35.53</v>
       </c>
     </row>
-    <row r="545" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A545">
         <v>69.099999999999994</v>
       </c>
@@ -12776,7 +12741,7 @@
         <v>35.454000000000001</v>
       </c>
     </row>
-    <row r="546" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A546">
         <v>76.8</v>
       </c>
@@ -12802,7 +12767,7 @@
         <v>35.219000000000001</v>
       </c>
     </row>
-    <row r="547" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A547">
         <v>84.4</v>
       </c>
@@ -12828,7 +12793,7 @@
         <v>35.247</v>
       </c>
     </row>
-    <row r="548" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A548">
         <v>92.1</v>
       </c>
@@ -12854,7 +12819,7 @@
         <v>34.648000000000003</v>
       </c>
     </row>
-    <row r="549" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A549">
         <v>99.8</v>
       </c>
@@ -12880,7 +12845,7 @@
         <v>34.491999999999997</v>
       </c>
     </row>
-    <row r="550" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A550">
         <v>107.5</v>
       </c>
@@ -12906,7 +12871,7 @@
         <v>34.625</v>
       </c>
     </row>
-    <row r="551" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A551">
         <v>115.1</v>
       </c>
@@ -12932,7 +12897,7 @@
         <v>34.369</v>
       </c>
     </row>
-    <row r="552" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A552">
         <v>122.8</v>
       </c>
@@ -12958,7 +12923,7 @@
         <v>34.036999999999999</v>
       </c>
     </row>
-    <row r="553" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A553">
         <v>130.5</v>
       </c>
@@ -12984,7 +12949,7 @@
         <v>33.42</v>
       </c>
     </row>
-    <row r="554" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A554">
         <v>138.19999999999999</v>
       </c>
@@ -13010,7 +12975,7 @@
         <v>32.109000000000002</v>
       </c>
     </row>
-    <row r="555" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A555">
         <v>145.9</v>
       </c>
@@ -13036,7 +13001,7 @@
         <v>30.305</v>
       </c>
     </row>
-    <row r="556" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A556">
         <v>153.5</v>
       </c>
@@ -13062,7 +13027,7 @@
         <v>27.843</v>
       </c>
     </row>
-    <row r="557" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A557">
         <v>161.19999999999999</v>
       </c>
@@ -13088,7 +13053,7 @@
         <v>24.898</v>
       </c>
     </row>
-    <row r="558" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A558">
         <v>168.9</v>
       </c>
@@ -13114,7 +13079,7 @@
         <v>22.597999999999999</v>
       </c>
     </row>
-    <row r="559" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A559">
         <v>176.6</v>
       </c>
@@ -13140,7 +13105,7 @@
         <v>19.603999999999999</v>
       </c>
     </row>
-    <row r="560" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A560">
         <v>184.2</v>
       </c>
@@ -13166,7 +13131,7 @@
         <v>16.431000000000001</v>
       </c>
     </row>
-    <row r="561" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A561">
         <v>191.9</v>
       </c>
@@ -13192,35 +13157,33 @@
         <v>12.968</v>
       </c>
     </row>
-    <row r="562" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A562">
         <v>199.6</v>
       </c>
-      <c r="B562" t="s">
-        <v>48</v>
-      </c>
-      <c r="C562" t="e" cm="1">
-        <f t="array" ref="C562">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D562" t="e" cm="1">
-        <f t="array" ref="D562">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E562" t="e" cm="1">
-        <f t="array" ref="E562">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F562" t="e" cm="1">
-        <f t="array" ref="F562">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G562" t="e" cm="1">
-        <f t="array" ref="G562">-NaN</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="563" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B562">
+        <v>0.94</v>
+      </c>
+      <c r="C562">
+        <v>0</v>
+      </c>
+      <c r="D562">
+        <v>0</v>
+      </c>
+      <c r="E562">
+        <v>0</v>
+      </c>
+      <c r="F562">
+        <v>0</v>
+      </c>
+      <c r="G562">
+        <v>0</v>
+      </c>
+      <c r="H562">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A563">
         <v>207.3</v>
       </c>
@@ -13246,7 +13209,7 @@
         <v>5.3769999999999998</v>
       </c>
     </row>
-    <row r="564" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A564">
         <v>214.9</v>
       </c>
@@ -13272,7 +13235,7 @@
         <v>2.5619999999999998</v>
       </c>
     </row>
-    <row r="565" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A565">
         <v>222.6</v>
       </c>

</xml_diff>